<commit_message>
Script triggers inside tables #74
</commit_message>
<xml_diff>
--- a/SQLCompare.Test/Datasources/ScriptMicrosoftSqlDataTypeTest.xlsx
+++ b/SQLCompare.Test/Datasources/ScriptMicrosoftSqlDataTypeTest.xlsx
@@ -174,12 +174,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">CREATE TYPE [TestSchema].[custom_nvarchar]
-    FROM nvarchar(555) NOT NULL
-GO
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">CREATE TYPE [TestSchema].[custom_char]
     FROM char(456) NOT NULL
 GO
@@ -210,12 +204,6 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">CREATE TYPE [TestSchema].[custom_nchar]
-    FROM nchar(9) NULL
-GO
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">CREATE TYPE [TestSchema].[custom_numeric]
     FROM numeric(20,10) NULL
 GO
@@ -236,6 +224,18 @@
   <si>
     <t xml:space="preserve">CREATE TYPE [TestSchema].[custom_time]
     FROM time(4) NULL
+GO
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CREATE TYPE [TestSchema].[custom_nvarchar]
+    FROM nvarchar(250) NOT NULL
+GO
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CREATE TYPE [TestSchema].[custom_nchar]
+    FROM nchar(45) NULL
 GO
 </t>
   </si>
@@ -592,7 +592,7 @@
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="J1" sqref="J1"/>
-      <selection pane="bottomLeft" activeCell="J14" sqref="J14"/>
+      <selection pane="bottomLeft" activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -718,7 +718,7 @@
         <v>36</v>
       </c>
       <c r="J4" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -772,7 +772,7 @@
         <v>5</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -800,7 +800,7 @@
         <v>38</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -830,7 +830,7 @@
         <v>6</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -882,7 +882,7 @@
         <v>8</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -901,7 +901,7 @@
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
       <c r="G11" s="2">
-        <v>9</v>
+        <v>90</v>
       </c>
       <c r="H11" s="2" t="s">
         <v>18</v>
@@ -910,7 +910,7 @@
         <v>39</v>
       </c>
       <c r="J11" s="5" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -940,7 +940,7 @@
         <v>40</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -959,7 +959,7 @@
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
       <c r="G13" s="2">
-        <v>555</v>
+        <v>500</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>18</v>
@@ -968,7 +968,7 @@
         <v>9</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -996,7 +996,7 @@
         <v>9</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -1024,7 +1024,7 @@
         <v>41</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="60" x14ac:dyDescent="0.25">
@@ -1052,7 +1052,7 @@
         <v>10</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>